<commit_message>
add: Tugas Profile Picture management
</commit_message>
<xml_diff>
--- a/public/template_supplier.xlsx
+++ b/public/template_supplier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B414A073-D6F9-4B8D-81E3-C34B8E1E5CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38D3F43-0458-4D52-88FE-B90762819DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{3CEABA5A-144D-4645-B3F4-25680944643C}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{3CEABA5A-144D-4645-B3F4-25680944643C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>supplier_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>supplier_nama</t>
   </si>
@@ -414,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24ACD6E4-4453-426E-BD9A-55C14F7D25E8}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,7 +425,7 @@
     <col min="4" max="4" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,21 +435,15 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>90876767568</v>
       </c>
     </row>

</xml_diff>